<commit_message>
datatype error const to let
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">enrollmentNo</t>
   </si>
@@ -37,67 +37,70 @@
     <t xml:space="preserve">sgpa</t>
   </si>
   <si>
-    <t xml:space="preserve">1AUA22BIT001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1AUA22BIT019</t>
+    <t xml:space="preserve">OS</t>
   </si>
   <si>
     <t xml:space="preserve">1AUA22BIT020</t>
   </si>
   <si>
     <t xml:space="preserve">1AUA22BIT021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1AUA22BIT040</t>
   </si>
 </sst>
 </file>
@@ -208,13 +211,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
@@ -236,362 +239,428 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>220001</v>
+        <v>220020</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>220002</v>
+        <v>220021</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>220003</v>
+        <v>220022</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>220004</v>
+        <v>220023</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>220005</v>
+        <v>220024</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>220006</v>
+        <v>220025</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>6</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>220007</v>
+        <v>220026</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>7</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>220008</v>
+        <v>220027</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>220009</v>
+        <v>220028</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>9</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>220010</v>
+        <v>220029</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>220011</v>
+        <v>220030</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>11</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>220012</v>
+        <v>220031</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>220013</v>
+        <v>220032</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>13</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>220014</v>
+        <v>220033</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>14</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>220015</v>
+        <v>220034</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="F16" s="0" t="n">
         <v>15</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>220016</v>
+        <v>220035</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>16</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>220017</v>
+        <v>220036</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>17</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>220018</v>
+        <v>220037</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="F19" s="0" t="n">
         <v>18</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>220019</v>
+        <v>220038</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F20" s="0" t="n">
         <v>19</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>220020</v>
+        <v>220039</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>20</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>220021</v>
+        <v>220040</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="F22" s="0" t="n">
         <v>21</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>